<commit_message>
Small change to search overview data Add new line to say that for CENTRAL X were primary studies rather than reviews
</commit_message>
<xml_diff>
--- a/data/sys-rev/searchResults_19_06_03.xlsx
+++ b/data/sys-rev/searchResults_19_06_03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/lm16564_bristol_ac_uk/Documents/Documents/rrr/thesis/data/sys-rev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{559E830B-CBAD-4072-8724-F8BEEDB79277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09A83483-951D-48A6-AEAB-9D4567C90433}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{559E830B-CBAD-4072-8724-F8BEEDB79277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71B9AE31-F7FC-4F14-AD0B-797B616B897E}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="19185" windowHeight="10200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="406">
   <si>
     <t>dement*.ti,ab.</t>
   </si>
@@ -767,216 +767,6 @@
     <t>[mh "cognitive dysfunction"]</t>
   </si>
   <si>
-    <t>#1</t>
-  </si>
-  <si>
-    <t>#2</t>
-  </si>
-  <si>
-    <t>#3</t>
-  </si>
-  <si>
-    <t>#4</t>
-  </si>
-  <si>
-    <t>#5</t>
-  </si>
-  <si>
-    <t>#6</t>
-  </si>
-  <si>
-    <t>#7</t>
-  </si>
-  <si>
-    <t>#8</t>
-  </si>
-  <si>
-    <t>#9</t>
-  </si>
-  <si>
-    <t>#10</t>
-  </si>
-  <si>
-    <t>#11</t>
-  </si>
-  <si>
-    <t>#12</t>
-  </si>
-  <si>
-    <t>#13</t>
-  </si>
-  <si>
-    <t>#14</t>
-  </si>
-  <si>
-    <t>#15</t>
-  </si>
-  <si>
-    <t>#16</t>
-  </si>
-  <si>
-    <t>#17</t>
-  </si>
-  <si>
-    <t>#18</t>
-  </si>
-  <si>
-    <t>#19</t>
-  </si>
-  <si>
-    <t>#20</t>
-  </si>
-  <si>
-    <t>#21</t>
-  </si>
-  <si>
-    <t>#22</t>
-  </si>
-  <si>
-    <t>#23</t>
-  </si>
-  <si>
-    <t>#24</t>
-  </si>
-  <si>
-    <t>#25</t>
-  </si>
-  <si>
-    <t>#26</t>
-  </si>
-  <si>
-    <t>#27</t>
-  </si>
-  <si>
-    <t>#28</t>
-  </si>
-  <si>
-    <t>#29</t>
-  </si>
-  <si>
-    <t>#30</t>
-  </si>
-  <si>
-    <t>#31</t>
-  </si>
-  <si>
-    <t>#32</t>
-  </si>
-  <si>
-    <t>#33</t>
-  </si>
-  <si>
-    <t>#34</t>
-  </si>
-  <si>
-    <t>#35</t>
-  </si>
-  <si>
-    <t>#36</t>
-  </si>
-  <si>
-    <t>#37</t>
-  </si>
-  <si>
-    <t>#38</t>
-  </si>
-  <si>
-    <t>#39</t>
-  </si>
-  <si>
-    <t>#40</t>
-  </si>
-  <si>
-    <t>#41</t>
-  </si>
-  <si>
-    <t>#42</t>
-  </si>
-  <si>
-    <t>#43</t>
-  </si>
-  <si>
-    <t>#44</t>
-  </si>
-  <si>
-    <t>#45</t>
-  </si>
-  <si>
-    <t>#46</t>
-  </si>
-  <si>
-    <t>#47</t>
-  </si>
-  <si>
-    <t>#48</t>
-  </si>
-  <si>
-    <t>#49</t>
-  </si>
-  <si>
-    <t>#50</t>
-  </si>
-  <si>
-    <t>#51</t>
-  </si>
-  <si>
-    <t>#52</t>
-  </si>
-  <si>
-    <t>#53</t>
-  </si>
-  <si>
-    <t>#54</t>
-  </si>
-  <si>
-    <t>#55</t>
-  </si>
-  <si>
-    <t>#56</t>
-  </si>
-  <si>
-    <t>#57</t>
-  </si>
-  <si>
-    <t>#58</t>
-  </si>
-  <si>
-    <t>#59</t>
-  </si>
-  <si>
-    <t>#60</t>
-  </si>
-  <si>
-    <t>#61</t>
-  </si>
-  <si>
-    <t>#62</t>
-  </si>
-  <si>
-    <t>#63</t>
-  </si>
-  <si>
-    <t>#64</t>
-  </si>
-  <si>
-    <t>#65</t>
-  </si>
-  <si>
-    <t>#66</t>
-  </si>
-  <si>
-    <t>#67</t>
-  </si>
-  <si>
-    <t>#68</t>
-  </si>
-  <si>
-    <t>#69</t>
-  </si>
-  <si>
-    <t>#70</t>
-  </si>
-  <si>
     <t>((mild or slight) NEAR2 (cognitive or cognition) NEAR2 (disorder* or defect* or deficit* or disabilit* or dysfunction or impair*))</t>
   </si>
   <si>
@@ -1241,24 +1031,6 @@
     <t>(age-associated) NEAR2 (memory decline)</t>
   </si>
   <si>
-    <t>#71</t>
-  </si>
-  <si>
-    <t>#72</t>
-  </si>
-  <si>
-    <t>#73</t>
-  </si>
-  <si>
-    <t>#74</t>
-  </si>
-  <si>
-    <t>#75</t>
-  </si>
-  <si>
-    <t>#76</t>
-  </si>
-  <si>
     <t xml:space="preserve">#1 OR #2 OR #3 OR #4 OR #5 OR #6 or #7 or #8 or #9 or #10 or #11 OR #12 OR #13 OR #14 OR #15 OR #16 OR #17 </t>
   </si>
   <si>
@@ -1482,6 +1254,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Limiting to trials rather than reviews/protcols</t>
   </si>
 </sst>
 </file>
@@ -2078,64 +1853,64 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>460</v>
+        <v>384</v>
       </c>
       <c r="E1" t="s">
-        <v>459</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>461</v>
+        <v>385</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>457</v>
+        <v>381</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>458</v>
+        <v>382</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>451</v>
+        <v>375</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>456</v>
+        <v>380</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>454</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>430</v>
+        <v>354</v>
       </c>
       <c r="B3" s="32">
         <v>6045</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>437</v>
+        <v>361</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>452</v>
+        <v>376</v>
       </c>
       <c r="G3" s="32">
         <v>23447</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>452</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>431</v>
+        <v>355</v>
       </c>
       <c r="B4" s="32">
         <v>10255</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>438</v>
+        <v>362</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>445</v>
+        <v>369</v>
       </c>
       <c r="G4" s="32">
         <v>19424</v>
@@ -2146,16 +1921,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>432</v>
+        <v>356</v>
       </c>
       <c r="B5" s="32">
         <v>800</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>439</v>
+        <v>363</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>453</v>
+        <v>377</v>
       </c>
       <c r="G5" s="32">
         <v>18683</v>
@@ -2166,16 +1941,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>433</v>
+        <v>357</v>
       </c>
       <c r="B6" s="32">
         <v>1473</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>440</v>
+        <v>364</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>446</v>
+        <v>370</v>
       </c>
       <c r="G6" s="32">
         <v>17420</v>
@@ -2186,16 +1961,16 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
-        <v>434</v>
+        <v>358</v>
       </c>
       <c r="B7" s="37">
         <v>4874</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>441</v>
+        <v>365</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>448</v>
+        <v>372</v>
       </c>
       <c r="G7" s="32">
         <v>17119</v>
@@ -2206,17 +1981,17 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>437</v>
+        <v>361</v>
       </c>
       <c r="B8" s="38">
         <f>SUM(B3:B7)</f>
         <v>23447</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>442</v>
+        <v>366</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>447</v>
+        <v>371</v>
       </c>
       <c r="G8" s="32">
         <v>17011</v>
@@ -2227,16 +2002,16 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
-        <v>436</v>
+        <v>360</v>
       </c>
       <c r="B9" s="37">
         <v>-7338</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>443</v>
+        <v>367</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>449</v>
+        <v>373</v>
       </c>
       <c r="G9" s="32">
         <v>16112</v>
@@ -2247,16 +2022,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>455</v>
+        <v>379</v>
       </c>
       <c r="B10" s="38">
         <v>16109</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>444</v>
+        <v>368</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>450</v>
+        <v>374</v>
       </c>
       <c r="G10" s="32">
         <v>16109</v>
@@ -2275,7 +2050,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
@@ -2316,7 +2091,7 @@
       </c>
       <c r="D2" s="40"/>
       <c r="F2" s="8" t="s">
-        <v>419</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2350,7 +2125,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>352</v>
+        <v>282</v>
       </c>
       <c r="C5" s="10">
         <v>2794</v>
@@ -2363,7 +2138,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>353</v>
+        <v>283</v>
       </c>
       <c r="C6" s="10">
         <v>24</v>
@@ -2376,7 +2151,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>354</v>
+        <v>284</v>
       </c>
       <c r="C7" s="10">
         <v>1051</v>
@@ -2389,7 +2164,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>355</v>
+        <v>285</v>
       </c>
       <c r="C8" s="10">
         <v>0</v>
@@ -2402,7 +2177,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>356</v>
+        <v>286</v>
       </c>
       <c r="C9" s="10">
         <v>381</v>
@@ -2415,7 +2190,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>357</v>
+        <v>287</v>
       </c>
       <c r="C10" s="10">
         <v>11</v>
@@ -2521,13 +2296,13 @@
         <v>18</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>358</v>
+        <v>288</v>
       </c>
       <c r="C18" s="11">
         <v>407352</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>325</v>
+        <v>255</v>
       </c>
       <c r="F18" s="8"/>
     </row>
@@ -2542,7 +2317,7 @@
         <v>462968</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>319</v>
+        <v>249</v>
       </c>
       <c r="F19" s="8"/>
     </row>
@@ -2747,7 +2522,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>359</v>
+        <v>289</v>
       </c>
       <c r="C36" s="11">
         <v>777210</v>
@@ -3149,7 +2924,7 @@
         <v>134</v>
       </c>
       <c r="D68" s="39" t="s">
-        <v>327</v>
+        <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3205,13 +2980,13 @@
         <v>73</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>360</v>
+        <v>290</v>
       </c>
       <c r="C73" s="11">
         <v>138108</v>
       </c>
       <c r="D73" s="23" t="s">
-        <v>326</v>
+        <v>256</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3219,13 +2994,13 @@
         <v>74</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>361</v>
+        <v>291</v>
       </c>
       <c r="C74" s="12">
         <v>19659</v>
       </c>
       <c r="D74" s="39" t="s">
-        <v>322</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3233,7 +3008,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>362</v>
+        <v>292</v>
       </c>
       <c r="C75" s="12">
         <v>2287</v>
@@ -3245,7 +3020,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>363</v>
+        <v>293</v>
       </c>
       <c r="C76" s="11">
         <v>21029</v>
@@ -3271,13 +3046,13 @@
         <v>78</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>364</v>
+        <v>294</v>
       </c>
       <c r="C78" s="17">
         <v>18226</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>321</v>
+        <v>251</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -3347,7 +3122,7 @@
         <v>84</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>365</v>
+        <v>295</v>
       </c>
       <c r="C84" s="11">
         <v>2933516</v>
@@ -3493,13 +3268,13 @@
         <v>96</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>366</v>
+        <v>296</v>
       </c>
       <c r="C96" s="11">
         <v>1616814</v>
       </c>
       <c r="D96" s="39" t="s">
-        <v>323</v>
+        <v>253</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3507,7 +3282,7 @@
         <v>97</v>
       </c>
       <c r="B97" s="15" t="s">
-        <v>367</v>
+        <v>297</v>
       </c>
       <c r="C97" s="11">
         <v>4175140</v>
@@ -3525,7 +3300,7 @@
         <v>736</v>
       </c>
       <c r="D98" s="39" t="s">
-        <v>320</v>
+        <v>250</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3545,7 +3320,7 @@
         <v>100</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>368</v>
+        <v>298</v>
       </c>
       <c r="C100" s="11">
         <v>1738</v>
@@ -3629,7 +3404,7 @@
         <v>107</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>369</v>
+        <v>299</v>
       </c>
       <c r="C107" s="11">
         <v>1894420</v>
@@ -3641,7 +3416,7 @@
         <v>108</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>370</v>
+        <v>300</v>
       </c>
       <c r="C108" s="12">
         <v>313</v>
@@ -3761,7 +3536,7 @@
         <v>118</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>376</v>
+        <v>306</v>
       </c>
       <c r="C118" s="11">
         <v>1768577</v>
@@ -3773,7 +3548,7 @@
         <v>119</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>372</v>
+        <v>302</v>
       </c>
       <c r="C119" s="12">
         <v>273</v>
@@ -3785,7 +3560,7 @@
         <v>120</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>373</v>
+        <v>303</v>
       </c>
       <c r="C120" s="12">
         <v>27</v>
@@ -3797,7 +3572,7 @@
         <v>121</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>375</v>
+        <v>305</v>
       </c>
       <c r="C121" s="11">
         <v>277</v>
@@ -3809,13 +3584,13 @@
         <v>122</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>374</v>
+        <v>304</v>
       </c>
       <c r="C122" s="11">
         <v>4175143</v>
       </c>
       <c r="D122" s="21" t="s">
-        <v>324</v>
+        <v>254</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3823,17 +3598,22 @@
         <v>123</v>
       </c>
       <c r="B123" s="18" t="s">
-        <v>377</v>
+        <v>307</v>
       </c>
       <c r="C123" s="17">
         <v>6045</v>
       </c>
       <c r="D123" s="27" t="s">
-        <v>328</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D98:D121"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="D74:D76"/>
+    <mergeCell ref="D79:D83"/>
+    <mergeCell ref="D85:D95"/>
     <mergeCell ref="D1:D10"/>
     <mergeCell ref="D11:D17"/>
     <mergeCell ref="D19:D35"/>
@@ -3843,11 +3623,6 @@
     <mergeCell ref="D46:D53"/>
     <mergeCell ref="D54:D57"/>
     <mergeCell ref="D58:D60"/>
-    <mergeCell ref="D98:D121"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="D74:D76"/>
-    <mergeCell ref="D79:D83"/>
-    <mergeCell ref="D85:D95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3896,7 +3671,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="F2" t="s">
-        <v>422</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3928,7 +3703,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>352</v>
+        <v>282</v>
       </c>
       <c r="C5" s="10">
         <v>3399</v>
@@ -3940,7 +3715,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>353</v>
+        <v>283</v>
       </c>
       <c r="C6" s="10">
         <v>52</v>
@@ -3952,7 +3727,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>354</v>
+        <v>284</v>
       </c>
       <c r="C7" s="10">
         <v>1877</v>
@@ -3964,7 +3739,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>355</v>
+        <v>285</v>
       </c>
       <c r="C8" s="10">
         <v>0</v>
@@ -3976,7 +3751,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>356</v>
+        <v>286</v>
       </c>
       <c r="C9" s="10">
         <v>714</v>
@@ -3988,7 +3763,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>357</v>
+        <v>287</v>
       </c>
       <c r="C10" s="10">
         <v>17</v>
@@ -4084,7 +3859,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>358</v>
+        <v>288</v>
       </c>
       <c r="C18" s="11">
         <v>613530</v>
@@ -4303,7 +4078,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>359</v>
+        <v>289</v>
       </c>
       <c r="C36" s="11">
         <v>1045396</v>
@@ -4765,7 +4540,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>360</v>
+        <v>290</v>
       </c>
       <c r="C73" s="11">
         <v>204136</v>
@@ -4779,7 +4554,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>361</v>
+        <v>291</v>
       </c>
       <c r="C74" s="12">
         <v>36463</v>
@@ -4791,7 +4566,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>362</v>
+        <v>292</v>
       </c>
       <c r="C75" s="12">
         <v>6013</v>
@@ -4803,7 +4578,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>363</v>
+        <v>293</v>
       </c>
       <c r="C76" s="11">
         <v>40002</v>
@@ -4827,7 +4602,7 @@
         <v>78</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>364</v>
+        <v>294</v>
       </c>
       <c r="C78" s="17">
         <v>39778</v>
@@ -4899,7 +4674,7 @@
         <v>84</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>365</v>
+        <v>295</v>
       </c>
       <c r="C84" s="10">
         <v>3106288</v>
@@ -5043,7 +4818,7 @@
         <v>96</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>366</v>
+        <v>296</v>
       </c>
       <c r="C96" s="11">
         <v>1682845</v>
@@ -5055,7 +4830,7 @@
         <v>97</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>367</v>
+        <v>297</v>
       </c>
       <c r="C97" s="11">
         <v>4464235</v>
@@ -5091,7 +4866,7 @@
         <v>100</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>368</v>
+        <v>298</v>
       </c>
       <c r="C100" s="11">
         <v>2447</v>
@@ -5175,7 +4950,7 @@
         <v>107</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>369</v>
+        <v>299</v>
       </c>
       <c r="C107" s="11">
         <v>2561978</v>
@@ -5187,7 +4962,7 @@
         <v>108</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>370</v>
+        <v>300</v>
       </c>
       <c r="C108" s="12">
         <v>499</v>
@@ -5307,7 +5082,7 @@
         <v>118</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>371</v>
+        <v>301</v>
       </c>
       <c r="C118" s="11">
         <v>2325782</v>
@@ -5319,7 +5094,7 @@
         <v>119</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>372</v>
+        <v>302</v>
       </c>
       <c r="C119" s="12">
         <v>499</v>
@@ -5331,7 +5106,7 @@
         <v>120</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>373</v>
+        <v>303</v>
       </c>
       <c r="C120" s="12">
         <v>147</v>
@@ -5343,7 +5118,7 @@
         <v>121</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>375</v>
+        <v>305</v>
       </c>
       <c r="C121" s="11">
         <v>499</v>
@@ -5355,7 +5130,7 @@
         <v>122</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>374</v>
+        <v>304</v>
       </c>
       <c r="C122" s="11">
         <v>4464264</v>
@@ -5367,7 +5142,7 @@
         <v>123</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>377</v>
+        <v>307</v>
       </c>
       <c r="C123" s="17">
         <v>10255</v>
@@ -5433,7 +5208,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="F2" t="s">
-        <v>435</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5465,7 +5240,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>352</v>
+        <v>282</v>
       </c>
       <c r="C5" s="3">
         <v>595</v>
@@ -5477,7 +5252,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>353</v>
+        <v>283</v>
       </c>
       <c r="C6" s="3">
         <v>13</v>
@@ -5489,7 +5264,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>354</v>
+        <v>284</v>
       </c>
       <c r="C7" s="3">
         <v>791</v>
@@ -5501,7 +5276,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>355</v>
+        <v>285</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -5513,7 +5288,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>356</v>
+        <v>286</v>
       </c>
       <c r="C9" s="3">
         <v>270</v>
@@ -5525,7 +5300,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>357</v>
+        <v>287</v>
       </c>
       <c r="C10" s="3">
         <v>8</v>
@@ -5597,7 +5372,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>378</v>
+        <v>308</v>
       </c>
       <c r="C16" s="5">
         <v>215471</v>
@@ -5801,7 +5576,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>379</v>
+        <v>309</v>
       </c>
       <c r="C33" s="5">
         <v>18467</v>
@@ -6185,7 +5960,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>380</v>
+        <v>310</v>
       </c>
       <c r="C65" s="5">
         <v>5782</v>
@@ -6197,7 +5972,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>381</v>
+        <v>311</v>
       </c>
       <c r="C66" s="6">
         <v>3318</v>
@@ -6209,7 +5984,7 @@
         <v>67</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>382</v>
+        <v>312</v>
       </c>
       <c r="C67" s="6">
         <v>585</v>
@@ -6221,7 +5996,7 @@
         <v>68</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>383</v>
+        <v>313</v>
       </c>
       <c r="C68" s="5">
         <v>3682</v>
@@ -6245,7 +6020,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>384</v>
+        <v>314</v>
       </c>
       <c r="C70" s="16">
         <v>3680</v>
@@ -6317,7 +6092,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>385</v>
+        <v>315</v>
       </c>
       <c r="C76" s="5">
         <v>261952</v>
@@ -6437,7 +6212,7 @@
         <v>86</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>386</v>
+        <v>316</v>
       </c>
       <c r="C86" s="5">
         <v>159116</v>
@@ -6449,7 +6224,7 @@
         <v>87</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>387</v>
+        <v>317</v>
       </c>
       <c r="C87" s="5">
         <v>408627</v>
@@ -6521,7 +6296,7 @@
         <v>93</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>388</v>
+        <v>318</v>
       </c>
       <c r="C93" s="5">
         <v>181514</v>
@@ -6533,7 +6308,7 @@
         <v>94</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>389</v>
+        <v>319</v>
       </c>
       <c r="C94" s="6">
         <v>12</v>
@@ -6653,7 +6428,7 @@
         <v>104</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>390</v>
+        <v>320</v>
       </c>
       <c r="C104" s="5">
         <v>211022</v>
@@ -6665,7 +6440,7 @@
         <v>105</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>391</v>
+        <v>321</v>
       </c>
       <c r="C105" s="6">
         <v>11</v>
@@ -6677,7 +6452,7 @@
         <v>106</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>392</v>
+        <v>322</v>
       </c>
       <c r="C106" s="5">
         <v>408627</v>
@@ -6689,7 +6464,7 @@
         <v>107</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>393</v>
+        <v>323</v>
       </c>
       <c r="C107" s="16">
         <v>800</v>
@@ -6705,10 +6480,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71F68F8-6C0C-4D8F-816A-AF0AB82EED17}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B17"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6717,8 +6492,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>242</v>
+      <c r="A1" s="3">
+        <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>119</v>
@@ -6728,12 +6503,12 @@
       </c>
       <c r="D1" s="3"/>
       <c r="F1" t="s">
-        <v>417</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>243</v>
+      <c r="A2" s="3">
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>120</v>
@@ -6744,8 +6519,8 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>244</v>
+      <c r="A3" s="3">
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>136</v>
@@ -6756,8 +6531,8 @@
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>245</v>
+      <c r="A4" s="3">
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>141</v>
@@ -6768,11 +6543,11 @@
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>246</v>
+      <c r="A5" s="3">
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>394</v>
+        <v>324</v>
       </c>
       <c r="C5" s="3">
         <v>1059</v>
@@ -6780,11 +6555,11 @@
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>247</v>
+      <c r="A6" s="3">
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>395</v>
+        <v>325</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -6792,11 +6567,11 @@
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>248</v>
+      <c r="A7" s="3">
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>396</v>
+        <v>326</v>
       </c>
       <c r="C7" s="3">
         <v>115</v>
@@ -6804,11 +6579,11 @@
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>249</v>
+      <c r="A8" s="3">
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>397</v>
+        <v>327</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -6816,11 +6591,11 @@
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>250</v>
+      <c r="A9" s="3">
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>398</v>
+        <v>328</v>
       </c>
       <c r="C9" s="3">
         <v>68</v>
@@ -6828,11 +6603,11 @@
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>251</v>
+      <c r="A10" s="3">
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>399</v>
+        <v>329</v>
       </c>
       <c r="C10" s="3">
         <v>2696</v>
@@ -6840,11 +6615,11 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>252</v>
+      <c r="A11" s="3">
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>312</v>
+        <v>242</v>
       </c>
       <c r="C11" s="3">
         <v>136</v>
@@ -6852,11 +6627,11 @@
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>253</v>
+      <c r="A12" s="3">
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>313</v>
+        <v>243</v>
       </c>
       <c r="C12" s="3">
         <v>45</v>
@@ -6864,11 +6639,11 @@
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>254</v>
+      <c r="A13" s="3">
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>314</v>
+        <v>244</v>
       </c>
       <c r="C13" s="3">
         <v>2288</v>
@@ -6876,11 +6651,11 @@
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>255</v>
+      <c r="A14" s="3">
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>315</v>
+        <v>245</v>
       </c>
       <c r="C14" s="3">
         <v>14935</v>
@@ -6888,8 +6663,8 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>256</v>
+      <c r="A15" s="3">
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>239</v>
@@ -6900,8 +6675,8 @@
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>257</v>
+      <c r="A16" s="3">
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>240</v>
@@ -6912,8 +6687,8 @@
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>258</v>
+      <c r="A17" s="3">
+        <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>241</v>
@@ -6924,11 +6699,11 @@
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>259</v>
+      <c r="A18" s="5">
+        <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>406</v>
+        <v>330</v>
       </c>
       <c r="C18" s="5">
         <v>38448</v>
@@ -6936,8 +6711,8 @@
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>260</v>
+      <c r="A19" s="3">
+        <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>121</v>
@@ -6948,8 +6723,8 @@
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>261</v>
+      <c r="A20" s="3">
+        <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>122</v>
@@ -6960,8 +6735,8 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>262</v>
+      <c r="A21" s="3">
+        <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>123</v>
@@ -6972,8 +6747,8 @@
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>263</v>
+      <c r="A22" s="3">
+        <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>124</v>
@@ -6984,8 +6759,8 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>264</v>
+      <c r="A23" s="3">
+        <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>125</v>
@@ -6996,8 +6771,8 @@
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>265</v>
+      <c r="A24" s="3">
+        <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>126</v>
@@ -7008,8 +6783,8 @@
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>266</v>
+      <c r="A25" s="3">
+        <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>127</v>
@@ -7020,8 +6795,8 @@
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>267</v>
+      <c r="A26" s="3">
+        <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>128</v>
@@ -7032,8 +6807,8 @@
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>268</v>
+      <c r="A27" s="3">
+        <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>129</v>
@@ -7044,8 +6819,8 @@
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>269</v>
+      <c r="A28" s="3">
+        <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>130</v>
@@ -7056,8 +6831,8 @@
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>270</v>
+      <c r="A29" s="3">
+        <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>131</v>
@@ -7068,8 +6843,8 @@
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>271</v>
+      <c r="A30" s="3">
+        <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>132</v>
@@ -7080,8 +6855,8 @@
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>272</v>
+      <c r="A31" s="3">
+        <v>31</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>133</v>
@@ -7092,8 +6867,8 @@
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>273</v>
+      <c r="A32" s="3">
+        <v>32</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>134</v>
@@ -7104,8 +6879,8 @@
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>274</v>
+      <c r="A33" s="3">
+        <v>33</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>137</v>
@@ -7116,8 +6891,8 @@
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>275</v>
+      <c r="A34" s="3">
+        <v>34</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>138</v>
@@ -7128,8 +6903,8 @@
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>276</v>
+      <c r="A35" s="3">
+        <v>35</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>139</v>
@@ -7140,11 +6915,11 @@
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>277</v>
+      <c r="A36" s="5">
+        <v>36</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>407</v>
+        <v>331</v>
       </c>
       <c r="C36" s="5">
         <v>69284</v>
@@ -7152,8 +6927,8 @@
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>278</v>
+      <c r="A37" s="3">
+        <v>37</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>88</v>
@@ -7164,8 +6939,8 @@
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>279</v>
+      <c r="A38" s="3">
+        <v>38</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>68</v>
@@ -7176,8 +6951,8 @@
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>280</v>
+      <c r="A39" s="3">
+        <v>39</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>222</v>
@@ -7188,8 +6963,8 @@
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>281</v>
+      <c r="A40" s="3">
+        <v>40</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>71</v>
@@ -7200,8 +6975,8 @@
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>282</v>
+      <c r="A41" s="3">
+        <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>72</v>
@@ -7212,8 +6987,8 @@
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>283</v>
+      <c r="A42" s="3">
+        <v>42</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>69</v>
@@ -7224,8 +6999,8 @@
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>284</v>
+      <c r="A43" s="3">
+        <v>43</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>70</v>
@@ -7236,8 +7011,8 @@
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>285</v>
+      <c r="A44" s="3">
+        <v>44</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>89</v>
@@ -7248,8 +7023,8 @@
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>286</v>
+      <c r="A45" s="3">
+        <v>45</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>218</v>
@@ -7260,8 +7035,8 @@
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>287</v>
+      <c r="A46" s="3">
+        <v>46</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>73</v>
@@ -7272,8 +7047,8 @@
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>288</v>
+      <c r="A47" s="3">
+        <v>47</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>145</v>
@@ -7284,8 +7059,8 @@
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>289</v>
+      <c r="A48" s="3">
+        <v>48</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>74</v>
@@ -7296,8 +7071,8 @@
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>290</v>
+      <c r="A49" s="3">
+        <v>49</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>75</v>
@@ -7308,8 +7083,8 @@
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>291</v>
+      <c r="A50" s="3">
+        <v>50</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>76</v>
@@ -7320,8 +7095,8 @@
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>292</v>
+      <c r="A51" s="3">
+        <v>51</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>117</v>
@@ -7332,8 +7107,8 @@
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>293</v>
+      <c r="A52" s="3">
+        <v>52</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>118</v>
@@ -7344,8 +7119,8 @@
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>294</v>
+      <c r="A53" s="3">
+        <v>53</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>77</v>
@@ -7356,8 +7131,8 @@
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>295</v>
+      <c r="A54" s="3">
+        <v>54</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>146</v>
@@ -7368,8 +7143,8 @@
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>296</v>
+      <c r="A55" s="3">
+        <v>55</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>79</v>
@@ -7380,8 +7155,8 @@
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>297</v>
+      <c r="A56" s="3">
+        <v>56</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>80</v>
@@ -7392,8 +7167,8 @@
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>298</v>
+      <c r="A57" s="3">
+        <v>57</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>81</v>
@@ -7404,8 +7179,8 @@
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>299</v>
+      <c r="A58" s="3">
+        <v>58</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>82</v>
@@ -7416,8 +7191,8 @@
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>300</v>
+      <c r="A59" s="3">
+        <v>59</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>83</v>
@@ -7428,8 +7203,8 @@
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>301</v>
+      <c r="A60" s="3">
+        <v>60</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>84</v>
@@ -7440,8 +7215,8 @@
       <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>302</v>
+      <c r="A61" s="3">
+        <v>61</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>135</v>
@@ -7452,8 +7227,8 @@
       <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>303</v>
+      <c r="A62" s="3">
+        <v>62</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>78</v>
@@ -7464,8 +7239,8 @@
       <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>304</v>
+      <c r="A63" s="3">
+        <v>63</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>85</v>
@@ -7476,8 +7251,8 @@
       <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>305</v>
+      <c r="A64" s="3">
+        <v>64</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>86</v>
@@ -7488,8 +7263,8 @@
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>306</v>
+      <c r="A65" s="3">
+        <v>65</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>87</v>
@@ -7500,11 +7275,11 @@
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>307</v>
+      <c r="A66" s="3">
+        <v>66</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>316</v>
+        <v>246</v>
       </c>
       <c r="C66" s="3">
         <v>95</v>
@@ -7512,11 +7287,11 @@
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>308</v>
+      <c r="A67" s="3">
+        <v>67</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>317</v>
+        <v>247</v>
       </c>
       <c r="C67" s="3">
         <v>21</v>
@@ -7524,11 +7299,11 @@
       <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>309</v>
+      <c r="A68" s="3">
+        <v>68</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>318</v>
+        <v>248</v>
       </c>
       <c r="C68" s="3">
         <v>2</v>
@@ -7536,8 +7311,8 @@
       <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>310</v>
+      <c r="A69" s="3">
+        <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>142</v>
@@ -7548,8 +7323,8 @@
       <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>311</v>
+      <c r="A70" s="3">
+        <v>70</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>143</v>
@@ -7560,8 +7335,8 @@
       <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>400</v>
+      <c r="A71" s="3">
+        <v>71</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>140</v>
@@ -7572,8 +7347,8 @@
       <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>401</v>
+      <c r="A72" s="3">
+        <v>72</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>144</v>
@@ -7584,11 +7359,11 @@
       <c r="D72" s="3"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>402</v>
+      <c r="A73" s="5">
+        <v>73</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>408</v>
+        <v>332</v>
       </c>
       <c r="C73" s="5">
         <v>21694</v>
@@ -7596,11 +7371,11 @@
       <c r="D73" s="5"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>403</v>
+      <c r="A74" s="6">
+        <v>74</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>409</v>
+        <v>333</v>
       </c>
       <c r="C74" s="6">
         <v>1605</v>
@@ -7608,11 +7383,11 @@
       <c r="D74" s="6"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
-        <v>404</v>
+      <c r="A75" s="6">
+        <v>75</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>410</v>
+        <v>334</v>
       </c>
       <c r="C75" s="6">
         <v>727</v>
@@ -7620,17 +7395,26 @@
       <c r="D75" s="6"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
-        <v>405</v>
+      <c r="A76" s="16">
+        <v>76</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>416</v>
+        <v>340</v>
       </c>
       <c r="C76" s="16">
         <v>2025</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>418</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="16"/>
+      <c r="B77" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="C77" s="16">
+        <v>1473</v>
       </c>
     </row>
   </sheetData>
@@ -7643,7 +7427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3923E6FA-3B91-46DE-9957-3F1F409D7948}">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -7680,7 +7464,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="F2" s="28" t="s">
-        <v>423</v>
+        <v>347</v>
       </c>
       <c r="G2" s="20"/>
       <c r="L2" s="20"/>
@@ -7690,14 +7474,14 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>411</v>
+        <v>335</v>
       </c>
       <c r="C3" s="3">
         <v>8119</v>
       </c>
       <c r="D3" s="3"/>
       <c r="F3" s="29" t="s">
-        <v>424</v>
+        <v>348</v>
       </c>
       <c r="G3" s="20"/>
       <c r="L3" s="20"/>
@@ -7707,14 +7491,14 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>412</v>
+        <v>336</v>
       </c>
       <c r="C4" s="3">
         <v>39</v>
       </c>
       <c r="D4" s="3"/>
       <c r="F4" s="29" t="s">
-        <v>425</v>
+        <v>349</v>
       </c>
       <c r="G4" s="20"/>
       <c r="L4" s="20"/>
@@ -7724,14 +7508,14 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>413</v>
+        <v>337</v>
       </c>
       <c r="C5" s="3">
         <v>1992</v>
       </c>
       <c r="D5" s="3"/>
       <c r="F5" s="29" t="s">
-        <v>426</v>
+        <v>350</v>
       </c>
       <c r="L5" s="20"/>
     </row>
@@ -7740,14 +7524,14 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>414</v>
+        <v>338</v>
       </c>
       <c r="C6" s="3">
         <v>4</v>
       </c>
       <c r="D6" s="3"/>
       <c r="F6" s="29" t="s">
-        <v>427</v>
+        <v>351</v>
       </c>
       <c r="G6" s="20"/>
       <c r="L6" s="20"/>
@@ -7757,14 +7541,14 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>415</v>
+        <v>339</v>
       </c>
       <c r="C7" s="3">
         <v>1271</v>
       </c>
       <c r="D7" s="3"/>
       <c r="F7" s="29" t="s">
-        <v>428</v>
+        <v>352</v>
       </c>
       <c r="L7" s="20"/>
     </row>
@@ -7773,14 +7557,14 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>420</v>
+        <v>344</v>
       </c>
       <c r="C8" s="3">
         <v>16</v>
       </c>
       <c r="D8" s="3"/>
       <c r="F8" s="29" t="s">
-        <v>429</v>
+        <v>353</v>
       </c>
       <c r="G8" s="20"/>
       <c r="L8" s="20"/>
@@ -7790,7 +7574,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>464</v>
+        <v>388</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -7801,7 +7585,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>465</v>
+        <v>389</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -7813,7 +7597,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>462</v>
+        <v>386</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -7825,7 +7609,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>463</v>
+        <v>387</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -7837,7 +7621,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>480</v>
+        <v>404</v>
       </c>
       <c r="C13" s="5">
         <v>313381</v>
@@ -8045,7 +7829,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>471</v>
+        <v>395</v>
       </c>
       <c r="C28" s="5">
         <v>920847</v>
@@ -8425,7 +8209,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>466</v>
+        <v>390</v>
       </c>
       <c r="C57" s="5">
         <v>108179</v>
@@ -8438,7 +8222,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>467</v>
+        <v>391</v>
       </c>
       <c r="C58" s="6">
         <v>18165</v>
@@ -8451,7 +8235,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>468</v>
+        <v>392</v>
       </c>
       <c r="C59" s="6">
         <v>2038</v>
@@ -8464,7 +8248,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>469</v>
+        <v>393</v>
       </c>
       <c r="C60" s="16">
         <v>19123</v>
@@ -8477,7 +8261,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>421</v>
+        <v>345</v>
       </c>
       <c r="C61" s="3">
         <v>1065411</v>
@@ -8490,7 +8274,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>329</v>
+        <v>259</v>
       </c>
       <c r="C62" s="3">
         <v>4896813</v>
@@ -8503,7 +8287,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>330</v>
+        <v>260</v>
       </c>
       <c r="C63" s="3">
         <v>235118</v>
@@ -8516,7 +8300,7 @@
         <v>64</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>331</v>
+        <v>261</v>
       </c>
       <c r="C64" s="3">
         <v>326505</v>
@@ -8529,7 +8313,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>470</v>
+        <v>394</v>
       </c>
       <c r="C65" s="5">
         <v>4948637</v>
@@ -8542,7 +8326,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>332</v>
+        <v>262</v>
       </c>
       <c r="C66" s="3">
         <v>267207</v>
@@ -8555,7 +8339,7 @@
         <v>67</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>333</v>
+        <v>263</v>
       </c>
       <c r="C67" s="3">
         <v>412461</v>
@@ -8568,7 +8352,7 @@
         <v>68</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>334</v>
+        <v>264</v>
       </c>
       <c r="C68" s="3">
         <v>843224</v>
@@ -8581,7 +8365,7 @@
         <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>335</v>
+        <v>265</v>
       </c>
       <c r="C69" s="3">
         <v>706888</v>
@@ -8594,7 +8378,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>336</v>
+        <v>266</v>
       </c>
       <c r="C70" s="3">
         <v>240446</v>
@@ -8607,7 +8391,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>337</v>
+        <v>267</v>
       </c>
       <c r="C71" s="3">
         <v>1533550</v>
@@ -8620,7 +8404,7 @@
         <v>72</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>338</v>
+        <v>268</v>
       </c>
       <c r="C72" s="3">
         <v>462747</v>
@@ -8633,7 +8417,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>339</v>
+        <v>269</v>
       </c>
       <c r="C73" s="3">
         <v>20886</v>
@@ -8646,7 +8430,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>340</v>
+        <v>270</v>
       </c>
       <c r="C74" s="3">
         <v>268471</v>
@@ -8658,7 +8442,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>472</v>
+        <v>396</v>
       </c>
       <c r="C75" s="5">
         <v>2393217</v>
@@ -8671,7 +8455,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>473</v>
+        <v>397</v>
       </c>
       <c r="C76" s="5">
         <v>6616705</v>
@@ -8684,7 +8468,7 @@
         <v>77</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>341</v>
+        <v>271</v>
       </c>
       <c r="C77" s="3">
         <v>273</v>
@@ -8697,7 +8481,7 @@
         <v>78</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>342</v>
+        <v>272</v>
       </c>
       <c r="C78" s="3">
         <v>654068</v>
@@ -8710,7 +8494,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>343</v>
+        <v>273</v>
       </c>
       <c r="C79" s="3">
         <v>196151</v>
@@ -8722,7 +8506,7 @@
         <v>80</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>344</v>
+        <v>274</v>
       </c>
       <c r="C80" s="3">
         <v>242109</v>
@@ -8735,7 +8519,7 @@
         <v>81</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>474</v>
+        <v>398</v>
       </c>
       <c r="C81" s="5">
         <v>975661</v>
@@ -8748,7 +8532,7 @@
         <v>82</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>475</v>
+        <v>399</v>
       </c>
       <c r="C82" s="6">
         <v>40</v>
@@ -8761,7 +8545,7 @@
         <v>83</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>345</v>
+        <v>275</v>
       </c>
       <c r="C83" s="3">
         <v>55089</v>
@@ -8774,7 +8558,7 @@
         <v>84</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>346</v>
+        <v>276</v>
       </c>
       <c r="C84" s="3">
         <v>67811</v>
@@ -8787,7 +8571,7 @@
         <v>85</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>347</v>
+        <v>277</v>
       </c>
       <c r="C85" s="3">
         <v>394086</v>
@@ -8800,7 +8584,7 @@
         <v>86</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>348</v>
+        <v>278</v>
       </c>
       <c r="C86" s="3">
         <v>257979</v>
@@ -8813,7 +8597,7 @@
         <v>87</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>349</v>
+        <v>279</v>
       </c>
       <c r="C87" s="3">
         <v>841646</v>
@@ -8826,7 +8610,7 @@
         <v>88</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>350</v>
+        <v>280</v>
       </c>
       <c r="C88" s="3">
         <v>116352</v>
@@ -8838,7 +8622,7 @@
         <v>89</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>351</v>
+        <v>281</v>
       </c>
       <c r="C89" s="3">
         <v>898995</v>
@@ -8851,7 +8635,7 @@
         <v>90</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>476</v>
+        <v>400</v>
       </c>
       <c r="C90" s="5">
         <v>2342704</v>
@@ -8864,7 +8648,7 @@
         <v>91</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>477</v>
+        <v>401</v>
       </c>
       <c r="C91" s="6">
         <v>36</v>
@@ -8876,7 +8660,7 @@
         <v>92</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>478</v>
+        <v>402</v>
       </c>
       <c r="C92" s="5">
         <v>6616705</v>
@@ -8888,7 +8672,7 @@
         <v>93</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>479</v>
+        <v>403</v>
       </c>
       <c r="C93" s="16">
         <v>4874</v>
@@ -8902,6 +8686,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D7E5106EC868644C97BE1423FB14B5FC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee29dcfb84d60cfbaf358a204b7b3d6d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9659c222-2717-4db3-8983-7ab564b1a641" xmlns:ns3="00622392-4907-4d87-82b3-6335d3a6b428" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cc0b4786329d9f4c4de705d674e3981" ns2:_="" ns3:_="">
     <xsd:import namespace="9659c222-2717-4db3-8983-7ab564b1a641"/>
@@ -9106,22 +8905,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CEBD6E8-56F8-4B9A-886F-CBBC5F428973}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9659c222-2717-4db3-8983-7ab564b1a641"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="00622392-4907-4d87-82b3-6335d3a6b428"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BFEB83B-014B-4A46-BA91-C883BC1057FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{246EEE14-1633-4A06-883E-5414A055D819}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9138,29 +8947,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BFEB83B-014B-4A46-BA91-C883BC1057FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CEBD6E8-56F8-4B9A-886F-CBBC5F428973}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9659c222-2717-4db3-8983-7ab564b1a641"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="00622392-4907-4d87-82b3-6335d3a6b428"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>